<commit_message>
Uploading new data files.
</commit_message>
<xml_diff>
--- a/data/female_conditioning/ovod1/rawresults_1-4_ovod1_b2.xlsx
+++ b/data/female_conditioning/ovod1/rawresults_1-4_ovod1_b2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/gitmicrobe-impacts-on-dietary-choice-in-drosophila-melanogaster/data/female_conditioning/ovod1/block_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster3/data/female_conditioning/ovod1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B84E118-A797-CC4E-B4EA-7FC08AC6F9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B231D41-0706-7B41-AA34-2E8C61E5029A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="25600" windowHeight="20480" xr2:uid="{04BE3046-FD22-3B44-8D0A-27A79407E4F9}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="25600" windowHeight="19980" xr2:uid="{04BE3046-FD22-3B44-8D0A-27A79407E4F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6D976C-B10E-844A-A263-8B278CA2AE5E}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -523,10 +523,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -537,10 +537,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -551,10 +551,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -565,10 +565,10 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -579,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,10 +593,10 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -635,10 +635,10 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -649,10 +649,10 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,10 +663,10 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,10 +677,10 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -691,10 +691,10 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -705,10 +705,10 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -719,10 +719,10 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -733,10 +733,10 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -761,10 +761,10 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -831,10 +831,10 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -873,10 +873,10 @@
         <v>3</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -887,10 +887,10 @@
         <v>3</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -985,10 +985,10 @@
         <v>4</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1041,10 +1041,10 @@
         <v>4</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1055,10 +1055,10 @@
         <v>4</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1083,10 +1083,10 @@
         <v>5</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1097,10 +1097,10 @@
         <v>5</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1111,10 +1111,10 @@
         <v>5</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1139,10 +1139,10 @@
         <v>5</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1153,10 +1153,10 @@
         <v>5</v>
       </c>
       <c r="C52">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1167,10 +1167,10 @@
         <v>5</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1181,10 +1181,10 @@
         <v>5</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1195,10 +1195,10 @@
         <v>5</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1209,10 +1209,10 @@
         <v>5</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1223,10 +1223,10 @@
         <v>6</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1265,10 +1265,10 @@
         <v>6</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1279,10 +1279,10 @@
         <v>6</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1307,10 +1307,10 @@
         <v>6</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1321,10 +1321,10 @@
         <v>6</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1349,10 +1349,10 @@
         <v>6</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1363,10 +1363,10 @@
         <v>6</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1377,10 +1377,10 @@
         <v>7</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1405,10 +1405,10 @@
         <v>7</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1419,10 +1419,10 @@
         <v>7</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1433,10 +1433,10 @@
         <v>7</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1447,10 +1447,10 @@
         <v>7</v>
       </c>
       <c r="C73">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1461,10 +1461,10 @@
         <v>7</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1475,10 +1475,10 @@
         <v>7</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1489,10 +1489,10 @@
         <v>7</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>